<commit_message>
Next: More Moves -> swift surf
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Monster RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2835423F-A1C8-4F61-92DB-189BAC275E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A968D8B5-91C2-40F8-B625-C7C94D0AF4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <dimension ref="A4:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
AI In Progress 1
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Monster RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5517526D-58DA-40CA-8FAC-0CB541AA2B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929BCADE-BD35-40C8-B9FB-8BA33C87DCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,17 +260,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -288,13 +303,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,11 +687,11 @@
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -769,7 +784,7 @@
   <dimension ref="A4:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,44 +796,44 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -841,7 +856,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="1">
@@ -861,7 +876,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="1">
@@ -881,7 +896,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="1">
@@ -901,7 +916,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="1">
@@ -921,7 +936,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="1">
@@ -941,7 +956,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="1">
@@ -961,7 +976,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="1">
@@ -981,7 +996,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1">
@@ -1001,7 +1016,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="1">
@@ -1021,7 +1036,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="1">

</xml_diff>

<commit_message>
AI in progress. NEXT: fix targets
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Monster RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929BCADE-BD35-40C8-B9FB-8BA33C87DCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2554F283-C790-4210-91D9-EB3FE623A633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="83">
   <si>
     <t>atk</t>
   </si>
@@ -222,6 +223,69 @@
   </si>
   <si>
     <t>Bonfire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Action: Swift Surf</t>
+  </si>
+  <si>
+    <t>User: FoeGreen</t>
+  </si>
+  <si>
+    <t>Weight:2</t>
+  </si>
+  <si>
+    <t>Targets:</t>
+  </si>
+  <si>
+    <t>FoeGreen</t>
+  </si>
+  <si>
+    <t>Action: Bamboo Bash</t>
+  </si>
+  <si>
+    <t>Action: Fire Blitz</t>
+  </si>
+  <si>
+    <t>Weight:1</t>
+  </si>
+  <si>
+    <t>FoeRed</t>
+  </si>
+  <si>
+    <t>FoeBlue</t>
+  </si>
+  <si>
+    <t>Action: Natural Remedy</t>
+  </si>
+  <si>
+    <t>User: FoeRed</t>
+  </si>
+  <si>
+    <t>Action: Icicle Blade</t>
+  </si>
+  <si>
+    <t>Weight:3</t>
+  </si>
+  <si>
+    <t>Action: Sticky Sticks</t>
+  </si>
+  <si>
+    <t>Action: Healing Pulse</t>
+  </si>
+  <si>
+    <t>User: FoeBlue</t>
+  </si>
+  <si>
+    <t>Action: Fire Ball</t>
+  </si>
+  <si>
+    <t>Action: Bonfire</t>
   </si>
 </sst>
 </file>
@@ -303,13 +367,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,11 +751,11 @@
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -784,7 +848,7 @@
   <dimension ref="A4:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,44 +860,44 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -856,7 +920,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="1">
@@ -876,7 +940,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="1">
@@ -896,7 +960,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="1">
@@ -916,7 +980,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="1">
@@ -936,7 +1000,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B13" s="1">
@@ -956,7 +1020,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="1">
@@ -976,7 +1040,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="1">
@@ -996,7 +1060,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1">
@@ -1016,7 +1080,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="1">
@@ -1026,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>26</v>
@@ -1036,7 +1100,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="1">
@@ -1067,4 +1131,582 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA257DF1-37EF-49C0-905E-B864A09E4FBF}">
+  <dimension ref="B2:B113"/>
+  <sheetViews>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>